<commit_message>
feat: input files models
</commit_message>
<xml_diff>
--- a/src/input-files/clients.xlsx
+++ b/src/input-files/clients.xlsx
@@ -30,30 +30,12 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
   <si>
-    <t>Josemar</t>
-  </si>
-  <si>
     <t>Anderson</t>
   </si>
   <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Nif</t>
-  </si>
-  <si>
     <t>Phone</t>
   </si>
   <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t>Category</t>
-  </si>
-  <si>
-    <t>test@test.com</t>
-  </si>
-  <si>
     <t>private</t>
   </si>
   <si>
@@ -63,7 +45,25 @@
     <t>corporative</t>
   </si>
   <si>
-    <t>ander@gmail.com</t>
+    <t>Name*</t>
+  </si>
+  <si>
+    <t>Nif*</t>
+  </si>
+  <si>
+    <t>Email*</t>
+  </si>
+  <si>
+    <t>Category*</t>
+  </si>
+  <si>
+    <t>c1@client.com</t>
+  </si>
+  <si>
+    <t>c2@client.com</t>
+  </si>
+  <si>
+    <t>Unitel</t>
   </si>
 </sst>
 </file>
@@ -116,11 +116,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperligação" xfId="1" builtinId="8"/>
@@ -405,64 +407,66 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="2" max="2" width="9.140625" style="5"/>
+    <col min="3" max="3" width="7" style="5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2">
+        <v>11</v>
+      </c>
+      <c r="B2" s="5">
         <v>356363</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="5">
         <v>363636</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E2" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="B3" s="5">
         <v>18</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="5">
         <v>557537</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E3" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -495,20 +499,21 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
+  <sheetProtection algorithmName="SHA-512" hashValue="ojuBrOKBV7v/Vj7oce1Z364T2t4DVOiVP4vVatmhSflmrMsM6PgyJfuIH60c2LX8tRU13AWNZ2NU/vk9H79wqw==" saltValue="rhZgnuby8CIpeaOL4hXQew==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>